<commit_message>
implement parallelized vgg16 and vgg19
</commit_message>
<xml_diff>
--- a/DL_config.xlsx
+++ b/DL_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zunzzz\Desktop\PCNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC490A0-8F61-49CA-B21D-6DFEFF1E85D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF42679-E14B-4071-BED5-210FDFBB4145}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YOLOv2" sheetId="1" r:id="rId1"/>
@@ -2600,8 +2600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
@@ -3320,8 +3320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="86" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
@@ -4672,17 +4672,6 @@
         <f>I19*J19*K19</f>
         <v>25088</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
       <c r="K20">
         <v>4096</v>
       </c>
@@ -4717,17 +4706,6 @@
         <f t="shared" si="9"/>
         <v>4096</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
       <c r="K21">
         <v>4096</v>
       </c>
@@ -4761,17 +4739,6 @@
       <c r="F22">
         <f t="shared" si="9"/>
         <v>4096</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="11"/>
-        <v>1</v>
       </c>
       <c r="K22">
         <v>1000</v>
@@ -4804,7 +4771,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="G23" sqref="G23:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>

</xml_diff>